<commit_message>
tarea resolucion parte 1
</commit_message>
<xml_diff>
--- a/Clase 2.xlsx
+++ b/Clase 2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB-USR-I-NS125-A302\Desktop\.NET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultimate\Desktop\.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>ENTRADA</t>
   </si>
@@ -72,6 +72,105 @@
   </si>
   <si>
     <t>preciofinal= ((1+ 0.35)12)*montoinicial</t>
+  </si>
+  <si>
+    <t>EJERCICIO 3</t>
+  </si>
+  <si>
+    <t>EJERCICIO 6</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>descuento= costo*0.05</t>
+  </si>
+  <si>
+    <t>costo inicial = hora *15</t>
+  </si>
+  <si>
+    <t>costo inicial</t>
+  </si>
+  <si>
+    <t>descuento</t>
+  </si>
+  <si>
+    <t>EJERCICIO 9</t>
+  </si>
+  <si>
+    <t>Deposito</t>
+  </si>
+  <si>
+    <t>computacion=(deposito*0.4)/2</t>
+  </si>
+  <si>
+    <t>administracion=(deposito * 0.5)/2</t>
+  </si>
+  <si>
+    <t>contabilidad=(deposito *0.7)/2</t>
+  </si>
+  <si>
+    <t>diseño= deposito - (computacion+administracion+contabilidad)</t>
+  </si>
+  <si>
+    <t>CONDICIONALES</t>
+  </si>
+  <si>
+    <t>ingreso</t>
+  </si>
+  <si>
+    <t>acumulado = ingreso * horas</t>
+  </si>
+  <si>
+    <t>descuento = 0.1*acumulado</t>
+  </si>
+  <si>
+    <t>montofinal = acumulado -descuento</t>
+  </si>
+  <si>
+    <t>HORA</t>
+  </si>
+  <si>
+    <t>acumulado &gt;1800</t>
+  </si>
+  <si>
+    <t>sueldo</t>
+  </si>
+  <si>
+    <t>bonificacion=(0.3 * sueldo)</t>
+  </si>
+  <si>
+    <t>asignacionfamiliar = (0.1 *sueldo)</t>
+  </si>
+  <si>
+    <t>total= bonificacion +asignacionfamiliar+sueldo</t>
+  </si>
+  <si>
+    <t>CURSO</t>
+  </si>
+  <si>
+    <t>nota 1</t>
+  </si>
+  <si>
+    <t>nota 2</t>
+  </si>
+  <si>
+    <t>nota 3</t>
+  </si>
+  <si>
+    <t>Promedio= nota 1+  nota 2+ nota 3</t>
+  </si>
+  <si>
+    <t>promedio &lt; 13.5</t>
+  </si>
+  <si>
+    <t>estado = desaprobado</t>
+  </si>
+  <si>
+    <t>promedio</t>
+  </si>
+  <si>
+    <t>estado</t>
   </si>
 </sst>
 </file>
@@ -101,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -124,16 +223,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -153,7 +295,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -228,6 +370,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -263,6 +422,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,28 +591,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -499,16 +675,16 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -566,12 +742,420 @@
       <c r="F8" s="1"/>
       <c r="H8" s="1"/>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <v>18000</v>
+      </c>
+      <c r="E15" s="1">
+        <f>(D15*0.4)/2</f>
+        <v>3600</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
+        <f>(D15*0.5)/2</f>
+        <v>4500</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <f>(D15*0.7)/2</f>
+        <v>6300</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1">
+        <f>D15-(SUM(E15:E17))</f>
+        <v>3600</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1">
+        <f>SUM(E15:E18)</f>
+        <v>18000</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1">
+        <v>20</v>
+      </c>
+      <c r="E29" s="1">
+        <f>(0.3*D29)</f>
+        <v>6</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1">
+        <f>(0.1 *D29)</f>
+        <v>2</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1">
+        <f>D29+E29+E30</f>
+        <v>28</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="13">
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>